<commit_message>
Mark FED VP and VAP+ as being part of F&E, and NPF not, in source SIT.
</commit_message>
<xml_diff>
--- a/sits/msit_feds.xlsx
+++ b/sits/msit_feds.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1815" uniqueCount="978">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1815" uniqueCount="979">
   <si>
     <t>Designation</t>
   </si>
@@ -2282,6 +2282,9 @@
       </rPr>
       <t xml:space="preserve">/3-4P</t>
     </r>
+  </si>
+  <si>
+    <t>F&amp;E (conjectural)</t>
   </si>
   <si>
     <t>Y181(B)</t>
@@ -4920,7 +4923,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right/>
@@ -4963,13 +4966,6 @@
       <bottom style="thick"/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
@@ -4996,7 +4992,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="35">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -5133,26 +5129,6 @@
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="6" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="6" fillId="0" fontId="6" numFmtId="165" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="6" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="6" fillId="0" fontId="6" numFmtId="165" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="6" fillId="0" fontId="6" numFmtId="166" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="true"/>
@@ -5176,8 +5152,8 @@
   </sheetPr>
   <dimension ref="A1:K246"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A210" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A215" activeCellId="0" pane="topLeft" sqref="215:216"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A97" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="L110" activeCellId="0" pane="topLeft" sqref="L110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -7172,7 +7148,7 @@
         <v>286</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>97</v>
+        <v>30</v>
       </c>
       <c r="E62" s="10" t="n">
         <v>1</v>
@@ -7207,7 +7183,7 @@
         <v>290</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>97</v>
+        <v>30</v>
       </c>
       <c r="E63" s="6" t="n">
         <v>1</v>
@@ -8737,33 +8713,33 @@
         <v>471</v>
       </c>
       <c r="D111" s="5" t="s">
-        <v>30</v>
+        <v>472</v>
       </c>
       <c r="E111" s="7" t="n">
         <v>6</v>
       </c>
       <c r="F111" s="5" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="G111" s="5" t="s">
         <v>394</v>
       </c>
       <c r="H111" s="5" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="I111" s="5" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="J111" s="31" t="n">
         <v>1.25</v>
       </c>
       <c r="K111" s="8" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="112">
       <c r="A112" s="3" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="B112" s="3"/>
       <c r="C112" s="4"/>
@@ -8778,13 +8754,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="113">
       <c r="A113" s="8" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B113" s="12" t="n">
         <v>5</v>
       </c>
       <c r="C113" s="13" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="D113" s="8" t="s">
         <v>30</v>
@@ -8793,10 +8769,10 @@
         <v>6</v>
       </c>
       <c r="F113" s="8" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="G113" s="8" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="H113" s="8" t="s">
         <v>33</v>
@@ -8808,18 +8784,18 @@
         <v>1.5</v>
       </c>
       <c r="K113" s="8" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="114">
       <c r="A114" s="8" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="C114" s="11" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="D114" s="8" t="s">
         <v>90</v>
@@ -8831,27 +8807,27 @@
         <v>130</v>
       </c>
       <c r="G114" s="8" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="H114" s="8" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="I114" s="8" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="J114" s="14" t="n">
         <v>1.5</v>
       </c>
       <c r="K114" s="8" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="115">
       <c r="A115" s="8" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="C115" s="13" t="s">
         <v>142</v>
@@ -8866,30 +8842,30 @@
         <v>181</v>
       </c>
       <c r="G115" s="8" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="H115" s="8" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="I115" s="8" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="J115" s="30" t="n">
         <v>2.25</v>
       </c>
       <c r="K115" s="8" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="116">
       <c r="A116" s="8" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="B116" s="10" t="n">
         <v>31</v>
       </c>
       <c r="C116" s="8" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="D116" s="8" t="s">
         <v>97</v>
@@ -8898,13 +8874,13 @@
         <v>6</v>
       </c>
       <c r="F116" s="8" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="G116" s="8" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="H116" s="8" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="I116" s="8" t="s">
         <v>420</v>
@@ -8913,18 +8889,18 @@
         <v>1.5</v>
       </c>
       <c r="K116" s="8" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="117">
       <c r="A117" s="8" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B117" s="10" t="n">
         <v>39</v>
       </c>
       <c r="C117" s="11" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="D117" s="8" t="s">
         <v>90</v>
@@ -8933,33 +8909,33 @@
         <v>6</v>
       </c>
       <c r="F117" s="8" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="G117" s="8" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="H117" s="8" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="I117" s="8" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="J117" s="14" t="n">
         <v>1.5</v>
       </c>
       <c r="K117" s="8" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="118">
       <c r="A118" s="5" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B118" s="6" t="n">
         <v>40</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="D118" s="5" t="s">
         <v>90</v>
@@ -8971,30 +8947,30 @@
         <v>137</v>
       </c>
       <c r="G118" s="5" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="H118" s="5" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="I118" s="5" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="J118" s="9" t="n">
         <v>1.5</v>
       </c>
       <c r="K118" s="8" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="119">
       <c r="A119" s="5" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="B119" s="6" t="n">
         <v>89</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="D119" s="5" t="s">
         <v>14</v>
@@ -9006,30 +8982,30 @@
         <v>38</v>
       </c>
       <c r="G119" s="5" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="H119" s="5" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="I119" s="5" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="J119" s="9" t="n">
         <v>1.5</v>
       </c>
       <c r="K119" s="8" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="120">
       <c r="A120" s="8" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="B120" s="10" t="n">
         <v>15</v>
       </c>
       <c r="C120" s="11" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="D120" s="8" t="s">
         <v>30</v>
@@ -9041,13 +9017,13 @@
         <v>44</v>
       </c>
       <c r="G120" s="8" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="H120" s="8" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="I120" s="8" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="J120" s="14" t="n">
         <v>1.5</v>
@@ -9058,13 +9034,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="121">
       <c r="A121" s="5" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="B121" s="5" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="C121" s="11" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="D121" s="5" t="s">
         <v>90</v>
@@ -9076,30 +9052,30 @@
         <v>57</v>
       </c>
       <c r="G121" s="5" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="H121" s="8" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="I121" s="5" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="J121" s="9" t="n">
         <v>1.5</v>
       </c>
       <c r="K121" s="8" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="42.95" outlineLevel="0" r="122">
       <c r="A122" s="15" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="B122" s="16" t="n">
         <v>88</v>
       </c>
       <c r="C122" s="21" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="D122" s="15" t="s">
         <v>14</v>
@@ -9111,24 +9087,24 @@
         <v>64</v>
       </c>
       <c r="G122" s="15" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="H122" s="5" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="I122" s="8" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="J122" s="18" t="n">
         <v>1.5</v>
       </c>
       <c r="K122" s="8" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="123">
       <c r="A123" s="3" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="B123" s="3"/>
       <c r="C123" s="3"/>
@@ -9143,13 +9119,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="124">
       <c r="A124" s="8" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="B124" s="10" t="n">
         <v>85</v>
       </c>
       <c r="C124" s="8" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="D124" s="8" t="s">
         <v>14</v>
@@ -9161,30 +9137,30 @@
         <v>372</v>
       </c>
       <c r="G124" s="8" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="H124" s="8" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="I124" s="8" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="J124" s="14" t="n">
         <v>1.5</v>
       </c>
       <c r="K124" s="8" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="125">
       <c r="A125" s="8" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="B125" s="10" t="n">
         <v>85</v>
       </c>
       <c r="C125" s="11" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="D125" s="8" t="s">
         <v>14</v>
@@ -9196,30 +9172,30 @@
         <v>372</v>
       </c>
       <c r="G125" s="8" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="H125" s="8" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="I125" s="8" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="J125" s="14" t="n">
         <v>1.5</v>
       </c>
       <c r="K125" s="8" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="126">
       <c r="A126" s="5" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="B126" s="6" t="n">
         <v>85</v>
       </c>
       <c r="C126" s="5" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="D126" s="5" t="s">
         <v>14</v>
@@ -9231,24 +9207,24 @@
         <v>372</v>
       </c>
       <c r="G126" s="5" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="H126" s="8" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="I126" s="5" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="J126" s="9" t="n">
         <v>1.5</v>
       </c>
       <c r="K126" s="5" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="127">
       <c r="A127" s="8" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="B127" s="10" t="n">
         <v>85</v>
@@ -9266,24 +9242,24 @@
         <v>372</v>
       </c>
       <c r="G127" s="8" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="H127" s="8" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="I127" s="8" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="J127" s="14" t="n">
         <v>1.5</v>
       </c>
       <c r="K127" s="8" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="128">
       <c r="A128" s="3" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="B128" s="3"/>
       <c r="C128" s="4"/>
@@ -9298,13 +9274,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="129">
       <c r="A129" s="5" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="B129" s="7" t="n">
         <v>6</v>
       </c>
       <c r="C129" s="19" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="D129" s="5" t="s">
         <v>30</v>
@@ -9316,10 +9292,10 @@
         <v>131</v>
       </c>
       <c r="G129" s="5" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="H129" s="5" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="I129" s="5" t="s">
         <v>420</v>
@@ -9328,18 +9304,18 @@
         <v>1.5</v>
       </c>
       <c r="K129" s="5" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="130">
       <c r="A130" s="8" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="B130" s="12" t="n">
         <v>7</v>
       </c>
       <c r="C130" s="11" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="D130" s="8" t="s">
         <v>30</v>
@@ -9351,30 +9327,30 @@
         <v>131</v>
       </c>
       <c r="G130" s="8" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="H130" s="8" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="I130" s="8" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="J130" s="14" t="n">
         <v>1.5</v>
       </c>
       <c r="K130" s="8" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="131">
       <c r="A131" s="8" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="B131" s="8" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="C131" s="13" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="D131" s="8" t="s">
         <v>90</v>
@@ -9386,30 +9362,30 @@
         <v>38</v>
       </c>
       <c r="G131" s="8" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="H131" s="8" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="I131" s="8" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="J131" s="14" t="n">
         <v>1.5</v>
       </c>
       <c r="K131" s="8" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="132">
       <c r="A132" s="8" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="B132" s="10" t="n">
         <v>14</v>
       </c>
       <c r="C132" s="11" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="D132" s="8" t="s">
         <v>30</v>
@@ -9421,24 +9397,24 @@
         <v>38</v>
       </c>
       <c r="G132" s="8" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="H132" s="8" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="I132" s="8" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="J132" s="14" t="n">
         <v>1.5</v>
       </c>
       <c r="K132" s="8" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="133">
       <c r="A133" s="8" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="B133" s="10" t="n">
         <v>202</v>
@@ -9456,30 +9432,30 @@
         <v>114</v>
       </c>
       <c r="G133" s="8" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="H133" s="8" t="s">
         <v>17</v>
       </c>
       <c r="I133" s="8" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="J133" s="14" t="n">
         <v>2.5</v>
       </c>
       <c r="K133" s="8" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="134">
       <c r="A134" s="8" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="B134" s="10" t="n">
         <v>205</v>
       </c>
       <c r="C134" s="11" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="D134" s="8" t="s">
         <v>14</v>
@@ -9491,19 +9467,19 @@
         <v>125</v>
       </c>
       <c r="G134" s="8" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="H134" s="8" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="I134" s="8" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="J134" s="14" t="n">
         <v>2.5</v>
       </c>
       <c r="K134" s="8" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32.1" outlineLevel="0" r="135">
@@ -9543,7 +9519,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="136">
       <c r="A136" s="3" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="B136" s="3"/>
       <c r="C136" s="3"/>
@@ -9558,13 +9534,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="137">
       <c r="A137" s="8" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="B137" s="10" t="n">
         <v>65</v>
       </c>
       <c r="C137" s="13" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="D137" s="8" t="s">
         <v>97</v>
@@ -9576,30 +9552,30 @@
         <v>70</v>
       </c>
       <c r="G137" s="8" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="H137" s="8" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="I137" s="8" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="J137" s="14" t="n">
         <v>1</v>
       </c>
       <c r="K137" s="8" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="138">
       <c r="A138" s="8" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="B138" s="10" t="n">
         <v>68</v>
       </c>
       <c r="C138" s="11" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="D138" s="8" t="s">
         <v>97</v>
@@ -9611,30 +9587,30 @@
         <v>70</v>
       </c>
       <c r="G138" s="8" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="H138" s="8" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="I138" s="8" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="J138" s="14" t="n">
         <v>1</v>
       </c>
       <c r="K138" s="8" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="139">
       <c r="A139" s="8" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="B139" s="10" t="n">
         <v>66</v>
       </c>
       <c r="C139" s="11" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="D139" s="8" t="s">
         <v>97</v>
@@ -9646,30 +9622,30 @@
         <v>70</v>
       </c>
       <c r="G139" s="8" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="H139" s="8" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="I139" s="8" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="J139" s="14" t="n">
         <v>1</v>
       </c>
       <c r="K139" s="8" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="140">
       <c r="A140" s="8" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="B140" s="10" t="n">
         <v>69</v>
       </c>
       <c r="C140" s="8" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="D140" s="8" t="s">
         <v>90</v>
@@ -9681,30 +9657,30 @@
         <v>349</v>
       </c>
       <c r="G140" s="8" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="H140" s="8" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="I140" s="8" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="J140" s="14" t="n">
         <v>1</v>
       </c>
       <c r="K140" s="8" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="141">
       <c r="A141" s="8" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="B141" s="10" t="n">
         <v>83</v>
       </c>
       <c r="C141" s="8" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="D141" s="8" t="s">
         <v>14</v>
@@ -9716,30 +9692,30 @@
         <v>349</v>
       </c>
       <c r="G141" s="8" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="H141" s="8" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="I141" s="8" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="J141" s="14" t="n">
         <v>1</v>
       </c>
       <c r="K141" s="8" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="142">
       <c r="A142" s="8" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="B142" s="10" t="n">
         <v>102</v>
       </c>
       <c r="C142" s="11" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="D142" s="8" t="s">
         <v>63</v>
@@ -9751,30 +9727,30 @@
         <v>107</v>
       </c>
       <c r="G142" s="8" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="H142" s="8" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="I142" s="8" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="J142" s="14" t="n">
         <v>1</v>
       </c>
       <c r="K142" s="8" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="143">
       <c r="A143" s="8" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="B143" s="10" t="n">
         <v>102</v>
       </c>
       <c r="C143" s="11" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="D143" s="8" t="s">
         <v>14</v>
@@ -9786,30 +9762,30 @@
         <v>107</v>
       </c>
       <c r="G143" s="8" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="H143" s="8" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="I143" s="8" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="J143" s="14" t="n">
         <v>1</v>
       </c>
       <c r="K143" s="8" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="144">
       <c r="A144" s="8" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="B144" s="10" t="n">
         <v>81</v>
       </c>
       <c r="C144" s="8" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="D144" s="8" t="s">
         <v>97</v>
@@ -9821,24 +9797,24 @@
         <v>107</v>
       </c>
       <c r="G144" s="8" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="H144" s="8" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="I144" s="8" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="J144" s="14" t="n">
         <v>1.2</v>
       </c>
       <c r="K144" s="8" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="145">
       <c r="A145" s="3" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="B145" s="3"/>
       <c r="C145" s="3"/>
@@ -9853,13 +9829,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="146">
       <c r="A146" s="5" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="B146" s="6" t="n">
         <v>50</v>
       </c>
       <c r="C146" s="19" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="D146" s="5" t="s">
         <v>14</v>
@@ -9871,30 +9847,30 @@
         <v>70</v>
       </c>
       <c r="G146" s="5" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="H146" s="5" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="I146" s="8" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="J146" s="31" t="n">
         <v>0.75</v>
       </c>
       <c r="K146" s="8" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="147">
       <c r="A147" s="5" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="B147" s="5" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="C147" s="11" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="D147" s="5" t="s">
         <v>90</v>
@@ -9906,30 +9882,30 @@
         <v>70</v>
       </c>
       <c r="G147" s="5" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="H147" s="8" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="I147" s="8" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="J147" s="31" t="n">
         <v>0.75</v>
       </c>
       <c r="K147" s="5" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="148">
       <c r="A148" s="5" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="B148" s="5" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="C148" s="11" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="D148" s="5" t="s">
         <v>90</v>
@@ -9941,30 +9917,30 @@
         <v>70</v>
       </c>
       <c r="G148" s="5" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="H148" s="8" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="I148" s="8" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="J148" s="31" t="n">
         <v>0.75</v>
       </c>
       <c r="K148" s="5" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="149">
       <c r="A149" s="5" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="B149" s="5" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="C149" s="11" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="D149" s="5" t="s">
         <v>90</v>
@@ -9976,24 +9952,24 @@
         <v>70</v>
       </c>
       <c r="G149" s="5" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="H149" s="8" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="I149" s="8" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="J149" s="31" t="n">
         <v>0.75</v>
       </c>
       <c r="K149" s="5" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="150">
       <c r="A150" s="3" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="B150" s="4"/>
       <c r="C150" s="4"/>
@@ -10008,13 +9984,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="151">
       <c r="A151" s="8" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="B151" s="10" t="n">
         <v>25</v>
       </c>
       <c r="C151" s="13" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="D151" s="8" t="s">
         <v>30</v>
@@ -10023,36 +9999,36 @@
         <v>3</v>
       </c>
       <c r="F151" s="8" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="G151" s="8" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="H151" s="8" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="I151" s="8" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="J151" s="30" t="n">
         <v>0.75</v>
       </c>
       <c r="K151" s="8" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="152">
       <c r="A152" s="5" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="B152" s="6" t="n">
         <v>86</v>
       </c>
       <c r="C152" s="11" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="D152" s="5" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="E152" s="7" t="n">
         <v>4</v>
@@ -10061,33 +10037,33 @@
         <v>258</v>
       </c>
       <c r="G152" s="5" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="H152" s="5" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="I152" s="5" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="J152" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K152" s="8" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="153">
       <c r="A153" s="8" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="B153" s="10" t="n">
         <v>47</v>
       </c>
       <c r="C153" s="8" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="D153" s="8" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="E153" s="12" t="n">
         <v>3</v>
@@ -10096,30 +10072,30 @@
         <v>137</v>
       </c>
       <c r="G153" s="8" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="H153" s="8" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="I153" s="8" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="J153" s="30" t="n">
         <v>0.75</v>
       </c>
       <c r="K153" s="8" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="154">
       <c r="A154" s="5" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="B154" s="6" t="n">
         <v>47</v>
       </c>
       <c r="C154" s="5" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="D154" s="5" t="s">
         <v>90</v>
@@ -10131,30 +10107,30 @@
         <v>137</v>
       </c>
       <c r="G154" s="5" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="H154" s="5" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="I154" s="5" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="J154" s="31" t="n">
         <v>0.75</v>
       </c>
       <c r="K154" s="5" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="155">
       <c r="A155" s="8" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="B155" s="10" t="n">
         <v>80</v>
       </c>
       <c r="C155" s="8" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="D155" s="8" t="s">
         <v>97</v>
@@ -10163,33 +10139,33 @@
         <v>3</v>
       </c>
       <c r="F155" s="8" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="G155" s="8" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="H155" s="8" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="I155" s="8" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="J155" s="30" t="n">
         <v>0.75</v>
       </c>
       <c r="K155" s="8" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="156">
       <c r="A156" s="8" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="B156" s="10" t="n">
         <v>41</v>
       </c>
       <c r="C156" s="11" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="D156" s="8" t="s">
         <v>30</v>
@@ -10201,30 +10177,30 @@
         <v>38</v>
       </c>
       <c r="G156" s="8" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="H156" s="8" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="I156" s="8" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="J156" s="30" t="n">
         <v>0.75</v>
       </c>
       <c r="K156" s="8" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="157">
       <c r="A157" s="8" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="B157" s="10" t="n">
         <v>44</v>
       </c>
       <c r="C157" s="11" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="D157" s="8" t="s">
         <v>30</v>
@@ -10236,30 +10212,30 @@
         <v>176</v>
       </c>
       <c r="G157" s="8" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="H157" s="8" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="I157" s="8" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="J157" s="30" t="n">
         <v>0.75</v>
       </c>
       <c r="K157" s="8" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="158">
       <c r="A158" s="5" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="B158" s="19" t="s">
         <v>49</v>
       </c>
       <c r="C158" s="8" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="D158" s="5" t="s">
         <v>30</v>
@@ -10283,18 +10259,18 @@
         <v>53</v>
       </c>
       <c r="K158" s="5" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="159">
       <c r="A159" s="8" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="B159" s="10" t="n">
         <v>49</v>
       </c>
       <c r="C159" s="8" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="D159" s="8" t="s">
         <v>30</v>
@@ -10306,30 +10282,30 @@
         <v>57</v>
       </c>
       <c r="G159" s="8" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="H159" s="8" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="I159" s="8" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="J159" s="30" t="n">
         <v>0.75</v>
       </c>
       <c r="K159" s="8" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="160">
       <c r="A160" s="8" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="B160" s="10" t="n">
         <v>84</v>
       </c>
       <c r="C160" s="11" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="D160" s="8" t="s">
         <v>14</v>
@@ -10341,24 +10317,24 @@
         <v>57</v>
       </c>
       <c r="G160" s="8" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="H160" s="8" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="I160" s="8" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="J160" s="30" t="n">
         <v>0.75</v>
       </c>
       <c r="K160" s="8" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="161">
       <c r="A161" s="8" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="B161" s="10" t="n">
         <v>203</v>
@@ -10376,24 +10352,24 @@
         <v>125</v>
       </c>
       <c r="G161" s="8" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="H161" s="8" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="I161" s="8" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="J161" s="30" t="n">
         <v>1.75</v>
       </c>
       <c r="K161" s="8" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="162">
       <c r="A162" s="3" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="B162" s="3"/>
       <c r="C162" s="4"/>
@@ -10408,13 +10384,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="163">
       <c r="A163" s="5" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="B163" s="6" t="n">
         <v>12</v>
       </c>
       <c r="C163" s="5" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="D163" s="5" t="s">
         <v>97</v>
@@ -10423,71 +10399,71 @@
         <v>3</v>
       </c>
       <c r="F163" s="5" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="G163" s="5" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H163" s="5" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="I163" s="8" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="J163" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K163" s="5" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="164">
       <c r="A164" s="8" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="B164" s="10" t="n">
         <v>137</v>
       </c>
       <c r="C164" s="8" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D164" s="8" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="E164" s="12" t="n">
         <v>4</v>
       </c>
       <c r="F164" s="8" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="G164" s="8" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H164" s="8" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="I164" s="8" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="J164" s="14" t="n">
         <v>0</v>
       </c>
       <c r="K164" s="8" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="165">
       <c r="A165" s="8" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="B165" s="10" t="n">
         <v>24</v>
       </c>
       <c r="C165" s="8" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="D165" s="8" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="E165" s="12" t="n">
         <v>4</v>
@@ -10496,24 +10472,24 @@
         <v>349</v>
       </c>
       <c r="G165" s="8" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H165" s="8" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="I165" s="8" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="J165" s="14" t="n">
         <v>0</v>
       </c>
       <c r="K165" s="8" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="166">
       <c r="A166" s="3" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="B166" s="3"/>
       <c r="C166" s="3"/>
@@ -10563,11 +10539,11 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="168">
       <c r="A168" s="8" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="B168" s="11"/>
       <c r="C168" s="13" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="D168" s="8" t="s">
         <v>14</v>
@@ -10582,21 +10558,21 @@
         <v>273</v>
       </c>
       <c r="H168" s="8" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="I168" s="8" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="J168" s="14" t="n">
         <v>0</v>
       </c>
       <c r="K168" s="8" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="169">
       <c r="A169" s="3" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="B169" s="3"/>
       <c r="C169" s="4"/>
@@ -10611,10 +10587,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="170">
       <c r="A170" s="8" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="B170" s="8" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="C170" s="8" t="s">
         <v>270</v>
@@ -10626,30 +10602,30 @@
         <v>0</v>
       </c>
       <c r="F170" s="8" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="G170" s="8" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="H170" s="8" t="s">
         <v>17</v>
       </c>
       <c r="I170" s="8" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="J170" s="14" t="n">
         <v>0</v>
       </c>
       <c r="K170" s="8" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="171">
       <c r="A171" s="5" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="B171" s="5" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="C171" s="5" t="s">
         <v>270</v>
@@ -10664,24 +10640,24 @@
         <v>107</v>
       </c>
       <c r="G171" s="5" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="H171" s="5" t="s">
         <v>17</v>
       </c>
       <c r="I171" s="5" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="J171" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K171" s="8" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="172">
       <c r="A172" s="33" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="B172" s="33"/>
       <c r="C172" s="33"/>
@@ -10696,13 +10672,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="173">
       <c r="A173" s="8" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="B173" s="8" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="C173" s="8" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="D173" s="8" t="s">
         <v>97</v>
@@ -10714,27 +10690,27 @@
         <v>137</v>
       </c>
       <c r="G173" s="8" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="H173" s="8" t="s">
         <v>17</v>
       </c>
       <c r="I173" s="8" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="J173" s="14" t="n">
         <v>2</v>
       </c>
       <c r="K173" s="8" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="174">
       <c r="A174" s="5" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="B174" s="8" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="C174" s="5" t="s">
         <v>286</v>
@@ -10749,62 +10725,62 @@
         <v>38</v>
       </c>
       <c r="G174" s="8" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="H174" s="5" t="s">
         <v>17</v>
       </c>
       <c r="I174" s="5" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="J174" s="9" t="n">
         <v>0.5</v>
       </c>
       <c r="K174" s="5" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="175">
       <c r="A175" s="8" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="B175" s="8" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="C175" s="5" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="D175" s="5" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="E175" s="6" t="n">
         <v>0</v>
       </c>
       <c r="F175" s="5" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="G175" s="8" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="H175" s="5" t="s">
         <v>17</v>
       </c>
       <c r="I175" s="5" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="J175" s="31" t="n">
         <v>0.75</v>
       </c>
       <c r="K175" s="5" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="176">
       <c r="A176" s="8" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="B176" s="8" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="C176" s="5" t="s">
         <v>290</v>
@@ -10816,27 +10792,27 @@
         <v>0</v>
       </c>
       <c r="F176" s="5" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="G176" s="8" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="H176" s="5" t="s">
         <v>17</v>
       </c>
       <c r="I176" s="5" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="J176" s="31" t="n">
         <v>1.25</v>
       </c>
       <c r="K176" s="5" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="177">
       <c r="A177" s="33" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="B177" s="33"/>
       <c r="C177" s="33"/>
@@ -10866,7 +10842,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="179">
       <c r="A179" s="33" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="B179" s="33"/>
       <c r="C179" s="33"/>
@@ -10881,13 +10857,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="180">
       <c r="A180" s="8" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="B180" s="10" t="n">
         <v>19</v>
       </c>
       <c r="C180" s="8" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="D180" s="8" t="s">
         <v>97</v>
@@ -10896,33 +10872,33 @@
         <v>0</v>
       </c>
       <c r="F180" s="8" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="G180" s="8" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="H180" s="8" t="s">
         <v>17</v>
       </c>
       <c r="I180" s="8" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="J180" s="14" t="n">
         <v>1</v>
       </c>
       <c r="K180" s="8" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="181">
       <c r="A181" s="8" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="B181" s="10" t="n">
         <v>62</v>
       </c>
       <c r="C181" s="8" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="D181" s="8" t="s">
         <v>90</v>
@@ -10931,33 +10907,33 @@
         <v>0</v>
       </c>
       <c r="F181" s="8" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="G181" s="8" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="H181" s="8" t="s">
         <v>17</v>
       </c>
       <c r="I181" s="8" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="J181" s="14" t="n">
         <v>1</v>
       </c>
       <c r="K181" s="8" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="182">
       <c r="A182" s="8" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="B182" s="10" t="n">
         <v>25</v>
       </c>
       <c r="C182" s="8" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="D182" s="8" t="s">
         <v>30</v>
@@ -10969,7 +10945,7 @@
         <v>271</v>
       </c>
       <c r="G182" s="8" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="H182" s="8" t="s">
         <v>273</v>
@@ -10981,18 +10957,18 @@
         <v>0</v>
       </c>
       <c r="K182" s="8" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="183">
       <c r="A183" s="8" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="B183" s="8" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="C183" s="11" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="D183" s="8" t="s">
         <v>14</v>
@@ -11004,30 +10980,30 @@
         <v>278</v>
       </c>
       <c r="G183" s="8" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="H183" s="8" t="s">
         <v>17</v>
       </c>
       <c r="I183" s="8" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="J183" s="14" t="n">
         <v>1</v>
       </c>
       <c r="K183" s="8" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="184">
       <c r="A184" s="8" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="B184" s="8" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="C184" s="8" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="D184" s="8" t="s">
         <v>97</v>
@@ -11039,30 +11015,30 @@
         <v>149</v>
       </c>
       <c r="G184" s="8" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="H184" s="8" t="s">
         <v>17</v>
       </c>
       <c r="I184" s="8" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="J184" s="14" t="n">
         <v>1</v>
       </c>
       <c r="K184" s="8" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="185">
       <c r="A185" s="5" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="B185" s="5" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="C185" s="11" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="D185" s="5" t="s">
         <v>14</v>
@@ -11071,33 +11047,33 @@
         <v>6</v>
       </c>
       <c r="F185" s="8" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="G185" s="5" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="H185" s="5" t="s">
         <v>17</v>
       </c>
       <c r="I185" s="5" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="J185" s="9" t="n">
         <v>1</v>
       </c>
       <c r="K185" s="8" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="186">
       <c r="A186" s="5" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="B186" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C186" s="5" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="D186" s="5" t="s">
         <v>21</v>
@@ -11106,33 +11082,33 @@
         <v>6</v>
       </c>
       <c r="F186" s="8" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="G186" s="5" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="H186" s="5" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="I186" s="5" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="J186" s="9" t="n">
         <v>1</v>
       </c>
       <c r="K186" s="5" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="187">
       <c r="A187" s="5" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="B187" s="6" t="n">
         <v>105</v>
       </c>
       <c r="C187" s="11" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="D187" s="5" t="s">
         <v>14</v>
@@ -11141,27 +11117,27 @@
         <v>6</v>
       </c>
       <c r="F187" s="8" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="G187" s="5" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="H187" s="5" t="s">
         <v>17</v>
       </c>
       <c r="I187" s="5" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="J187" s="9" t="n">
         <v>1</v>
       </c>
       <c r="K187" s="8" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="188">
       <c r="A188" s="33" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="B188" s="33"/>
       <c r="C188" s="33"/>
@@ -11176,13 +11152,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="189">
       <c r="A189" s="8" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="B189" s="10" t="n">
         <v>18</v>
       </c>
       <c r="C189" s="8" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="D189" s="8" t="s">
         <v>97</v>
@@ -11191,33 +11167,33 @@
         <v>0</v>
       </c>
       <c r="F189" s="8" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="G189" s="8" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="H189" s="8" t="s">
         <v>17</v>
       </c>
       <c r="I189" s="8" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="J189" s="14" t="n">
         <v>0.5</v>
       </c>
       <c r="K189" s="8" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="190">
       <c r="A190" s="8" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="B190" s="8" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="C190" s="11" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="D190" s="8" t="s">
         <v>14</v>
@@ -11229,30 +11205,30 @@
         <v>137</v>
       </c>
       <c r="G190" s="8" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="H190" s="8" t="s">
         <v>17</v>
       </c>
       <c r="I190" s="8" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="J190" s="14" t="n">
         <v>0.5</v>
       </c>
       <c r="K190" s="8" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="191">
       <c r="A191" s="8" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="B191" s="8" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="C191" s="8" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="D191" s="8" t="s">
         <v>97</v>
@@ -11264,30 +11240,30 @@
         <v>38</v>
       </c>
       <c r="G191" s="8" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="H191" s="8" t="s">
         <v>17</v>
       </c>
       <c r="I191" s="8" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="J191" s="14" t="n">
         <v>0.5</v>
       </c>
       <c r="K191" s="8" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="192">
       <c r="A192" s="5" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="B192" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C192" s="5" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="D192" s="5" t="s">
         <v>21</v>
@@ -11299,30 +11275,30 @@
         <v>70</v>
       </c>
       <c r="G192" s="5" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="H192" s="5" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="I192" s="5" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="J192" s="9" t="n">
         <v>0.5</v>
       </c>
       <c r="K192" s="5" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="193">
       <c r="A193" s="5" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="B193" s="5" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="C193" s="11" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="D193" s="5" t="s">
         <v>14</v>
@@ -11331,27 +11307,27 @@
         <v>3</v>
       </c>
       <c r="F193" s="8" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="G193" s="5" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="H193" s="5" t="s">
         <v>17</v>
       </c>
       <c r="I193" s="5" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="J193" s="9" t="n">
         <v>0.5</v>
       </c>
       <c r="K193" s="8" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="194">
       <c r="A194" s="33" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="B194" s="33"/>
       <c r="C194" s="33"/>
@@ -11366,13 +11342,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="195">
       <c r="A195" s="8" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="B195" s="12" t="n">
         <v>5</v>
       </c>
       <c r="C195" s="8" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="D195" s="8" t="s">
         <v>30</v>
@@ -11381,7 +11357,7 @@
         <v>0</v>
       </c>
       <c r="F195" s="8" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="G195" s="8" t="s">
         <v>273</v>
@@ -11390,24 +11366,24 @@
         <v>273</v>
       </c>
       <c r="I195" s="8" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="J195" s="14" t="n">
         <v>0</v>
       </c>
       <c r="K195" s="8" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="196">
       <c r="A196" s="8" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="B196" s="5" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="C196" s="5" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="D196" s="5" t="s">
         <v>97</v>
@@ -11416,7 +11392,7 @@
         <v>0</v>
       </c>
       <c r="F196" s="5" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="G196" s="5" t="s">
         <v>51</v>
@@ -11425,13 +11401,13 @@
         <v>17</v>
       </c>
       <c r="I196" s="8" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="J196" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K196" s="5" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32.1" outlineLevel="0" r="197">
@@ -11471,13 +11447,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="198">
       <c r="A198" s="5" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="B198" s="7" t="n">
         <v>8</v>
       </c>
       <c r="C198" s="5" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="D198" s="5" t="s">
         <v>90</v>
@@ -11486,33 +11462,33 @@
         <v>0</v>
       </c>
       <c r="F198" s="5" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="G198" s="5" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="H198" s="19" t="s">
         <v>17</v>
       </c>
       <c r="I198" s="5" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="J198" s="9" t="n">
         <v>0.2</v>
       </c>
       <c r="K198" s="8" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="199">
       <c r="A199" s="5" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="B199" s="6" t="n">
         <v>67</v>
       </c>
       <c r="C199" s="5" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="D199" s="5" t="s">
         <v>90</v>
@@ -11521,33 +11497,33 @@
         <v>3</v>
       </c>
       <c r="F199" s="5" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="G199" s="5" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="H199" s="5" t="s">
         <v>17</v>
       </c>
       <c r="I199" s="5" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="J199" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K199" s="8" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32.1" outlineLevel="0" r="200">
       <c r="A200" s="5" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="B200" s="6" t="n">
         <v>33</v>
       </c>
       <c r="C200" s="5" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="D200" s="5" t="s">
         <v>97</v>
@@ -11556,33 +11532,33 @@
         <v>0</v>
       </c>
       <c r="F200" s="5" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="G200" s="5" t="s">
         <v>51</v>
       </c>
       <c r="H200" s="8" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="I200" s="5" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="J200" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K200" s="5" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32.1" outlineLevel="0" r="201">
       <c r="A201" s="5" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="B201" s="6" t="n">
         <v>11</v>
       </c>
       <c r="C201" s="5" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="D201" s="5" t="s">
         <v>90</v>
@@ -11591,33 +11567,33 @@
         <v>0</v>
       </c>
       <c r="F201" s="5" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="G201" s="5" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="H201" s="5" t="s">
         <v>17</v>
       </c>
       <c r="I201" s="5" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="J201" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K201" s="8" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="202">
       <c r="A202" s="5" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="B202" s="5" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="C202" s="5" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="D202" s="5" t="s">
         <v>90</v>
@@ -11635,24 +11611,24 @@
         <v>273</v>
       </c>
       <c r="I202" s="5" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="J202" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K202" s="8" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="203">
       <c r="A203" s="8" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="B203" s="10" t="n">
         <v>20</v>
       </c>
       <c r="C203" s="8" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="D203" s="8" t="s">
         <v>14</v>
@@ -11670,24 +11646,24 @@
         <v>17</v>
       </c>
       <c r="I203" s="8" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="J203" s="14" t="n">
         <v>0</v>
       </c>
       <c r="K203" s="8" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="204">
       <c r="A204" s="5" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="B204" s="6" t="n">
         <v>45</v>
       </c>
       <c r="C204" s="22" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="D204" s="5" t="s">
         <v>90</v>
@@ -11699,30 +11675,30 @@
         <v>70</v>
       </c>
       <c r="G204" s="5" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="H204" s="5" t="s">
         <v>17</v>
       </c>
       <c r="I204" s="5" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="J204" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K204" s="8" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="205">
       <c r="A205" s="5" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="B205" s="5" t="s">
         <v>51</v>
       </c>
       <c r="C205" s="8" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="D205" s="5" t="s">
         <v>14</v>
@@ -11740,18 +11716,18 @@
         <v>17</v>
       </c>
       <c r="I205" s="5" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="J205" s="9" t="n">
         <v>6</v>
       </c>
       <c r="K205" s="5" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="206">
       <c r="A206" s="33" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="B206" s="33"/>
       <c r="C206" s="33"/>
@@ -11766,13 +11742,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="207">
       <c r="A207" s="8" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="B207" s="10" t="n">
         <v>10</v>
       </c>
       <c r="C207" s="8" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="D207" s="8" t="s">
         <v>30</v>
@@ -11781,33 +11757,33 @@
         <v>0</v>
       </c>
       <c r="F207" s="8" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="G207" s="8" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="H207" s="8" t="s">
         <v>273</v>
       </c>
       <c r="I207" s="8" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="J207" s="14" t="n">
         <v>0</v>
       </c>
       <c r="K207" s="8" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="208">
       <c r="A208" s="8" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="B208" s="10" t="n">
         <v>10</v>
       </c>
       <c r="C208" s="8" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="D208" s="8" t="s">
         <v>14</v>
@@ -11819,39 +11795,39 @@
         <v>149</v>
       </c>
       <c r="G208" s="8" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="H208" s="8" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="I208" s="8" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="J208" s="14" t="n">
         <v>0</v>
       </c>
       <c r="K208" s="8" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="209">
       <c r="A209" s="5" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="B209" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C209" s="5" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="D209" s="5" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="E209" s="7" t="n">
         <v>0</v>
       </c>
       <c r="F209" s="5" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="G209" s="5" t="s">
         <v>273</v>
@@ -11860,24 +11836,24 @@
         <v>273</v>
       </c>
       <c r="I209" s="5" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="J209" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K209" s="5" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="210">
       <c r="A210" s="5" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="B210" s="5" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="C210" s="5" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="D210" s="5" t="s">
         <v>14</v>
@@ -11889,24 +11865,24 @@
         <v>114</v>
       </c>
       <c r="G210" s="5" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="H210" s="5" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="I210" s="5" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="J210" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K210" s="5" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="211">
       <c r="A211" s="33" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="B211" s="33"/>
       <c r="C211" s="33"/>
@@ -11921,13 +11897,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="212">
       <c r="A212" s="8" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="B212" s="8" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="C212" s="11" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="D212" s="8" t="s">
         <v>97</v>
@@ -11936,13 +11912,13 @@
         <v>8</v>
       </c>
       <c r="F212" s="8" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="G212" s="8" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="H212" s="8" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="I212" s="8" t="s">
         <v>273</v>
@@ -11951,18 +11927,18 @@
         <v>0</v>
       </c>
       <c r="K212" s="8" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32.1" outlineLevel="0" r="213">
       <c r="A213" s="5" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="B213" s="7" t="n">
         <v>2</v>
       </c>
       <c r="C213" s="8" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="D213" s="5" t="s">
         <v>30</v>
@@ -11974,10 +11950,10 @@
         <v>308</v>
       </c>
       <c r="G213" s="5" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="H213" s="8" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="I213" s="5" t="s">
         <v>273</v>
@@ -11986,18 +11962,18 @@
         <v>0</v>
       </c>
       <c r="K213" s="5" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32.1" outlineLevel="0" r="214">
       <c r="A214" s="5" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="B214" s="7" t="n">
         <v>2</v>
       </c>
       <c r="C214" s="11" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="D214" s="5" t="s">
         <v>14</v>
@@ -12006,13 +11982,13 @@
         <v>9</v>
       </c>
       <c r="F214" s="5" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="G214" s="5" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="H214" s="8" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="I214" s="5" t="s">
         <v>273</v>
@@ -12021,88 +11997,88 @@
         <v>0</v>
       </c>
       <c r="K214" s="5" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="215">
-      <c r="A215" s="34" t="s">
-        <v>877</v>
-      </c>
-      <c r="B215" s="35" t="n">
+      <c r="A215" s="8" t="s">
+        <v>878</v>
+      </c>
+      <c r="B215" s="10" t="n">
         <v>24</v>
       </c>
-      <c r="C215" s="36" t="s">
+      <c r="C215" s="22" t="s">
         <v>270</v>
       </c>
-      <c r="D215" s="34" t="s">
+      <c r="D215" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="E215" s="37" t="n">
+      <c r="E215" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="F215" s="34" t="s">
-        <v>845</v>
-      </c>
-      <c r="G215" s="34" t="s">
-        <v>878</v>
-      </c>
-      <c r="H215" s="34" t="s">
+      <c r="F215" s="8" t="s">
+        <v>846</v>
+      </c>
+      <c r="G215" s="8" t="s">
+        <v>879</v>
+      </c>
+      <c r="H215" s="8" t="s">
         <v>273</v>
       </c>
-      <c r="I215" s="34" t="s">
-        <v>847</v>
-      </c>
-      <c r="J215" s="38" t="n">
+      <c r="I215" s="8" t="s">
+        <v>848</v>
+      </c>
+      <c r="J215" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="K215" s="34" t="s">
+      <c r="K215" s="8" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="216">
+      <c r="A216" s="8" t="s">
+        <v>881</v>
+      </c>
+      <c r="B216" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="C216" s="22" t="s">
+        <v>882</v>
+      </c>
+      <c r="D216" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E216" s="12" t="n">
+        <v>6</v>
+      </c>
+      <c r="F216" s="8" t="s">
+        <v>846</v>
+      </c>
+      <c r="G216" s="8" t="s">
         <v>879</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="216">
-      <c r="A216" s="34" t="s">
-        <v>880</v>
-      </c>
-      <c r="B216" s="35" t="n">
-        <v>24</v>
-      </c>
-      <c r="C216" s="36" t="s">
-        <v>881</v>
-      </c>
-      <c r="D216" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="E216" s="37" t="n">
-        <v>6</v>
-      </c>
-      <c r="F216" s="34" t="s">
-        <v>845</v>
-      </c>
-      <c r="G216" s="34" t="s">
-        <v>878</v>
-      </c>
-      <c r="H216" s="34" t="s">
+      <c r="H216" s="8" t="s">
         <v>273</v>
       </c>
-      <c r="I216" s="34" t="s">
+      <c r="I216" s="8" t="s">
         <v>273</v>
       </c>
-      <c r="J216" s="38" t="n">
+      <c r="J216" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="K216" s="34" t="s">
-        <v>882</v>
+      <c r="K216" s="8" t="s">
+        <v>883</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="217">
       <c r="A217" s="5" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="B217" s="5" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="C217" s="22" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="D217" s="5" t="s">
         <v>14</v>
@@ -12114,10 +12090,10 @@
         <v>137</v>
       </c>
       <c r="G217" s="5" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="H217" s="5" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="I217" s="5" t="s">
         <v>273</v>
@@ -12126,18 +12102,18 @@
         <v>0</v>
       </c>
       <c r="K217" s="8" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="218">
       <c r="A218" s="8" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="B218" s="12" t="n">
         <v>4</v>
       </c>
       <c r="C218" s="11" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="D218" s="8" t="s">
         <v>14</v>
@@ -12155,24 +12131,24 @@
         <v>17</v>
       </c>
       <c r="I218" s="8" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="J218" s="14" t="n">
         <v>0</v>
       </c>
       <c r="K218" s="8" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="219">
       <c r="A219" s="8" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="B219" s="8" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="C219" s="13" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="D219" s="8" t="s">
         <v>63</v>
@@ -12190,24 +12166,24 @@
         <v>17</v>
       </c>
       <c r="I219" s="8" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="J219" s="14" t="n">
         <v>0</v>
       </c>
       <c r="K219" s="8" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="220">
       <c r="A220" s="5" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="B220" s="6" t="n">
         <v>47</v>
       </c>
       <c r="C220" s="11" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="D220" s="5" t="s">
         <v>90</v>
@@ -12219,30 +12195,30 @@
         <v>70</v>
       </c>
       <c r="G220" s="5" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="H220" s="8" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="I220" s="5" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="J220" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K220" s="5" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="221">
       <c r="A221" s="8" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="B221" s="6" t="n">
         <v>17</v>
       </c>
       <c r="C221" s="19" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="D221" s="5" t="s">
         <v>14</v>
@@ -12260,24 +12236,24 @@
         <v>17</v>
       </c>
       <c r="I221" s="5" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="J221" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K221" s="5" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32.1" outlineLevel="0" r="222">
       <c r="A222" s="5" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="B222" s="6" t="n">
         <v>202</v>
       </c>
       <c r="C222" s="11" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="D222" s="5" t="s">
         <v>14</v>
@@ -12289,10 +12265,10 @@
         <v>114</v>
       </c>
       <c r="G222" s="5" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="H222" s="8" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="I222" s="5" t="s">
         <v>273</v>
@@ -12301,7 +12277,7 @@
         <v>0</v>
       </c>
       <c r="K222" s="5" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32.1" outlineLevel="0" r="223">
@@ -12341,13 +12317,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="224">
       <c r="A224" s="5" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="B224" s="5" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="C224" s="11" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="D224" s="5" t="s">
         <v>21</v>
@@ -12359,10 +12335,10 @@
         <v>114</v>
       </c>
       <c r="G224" s="5" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="H224" s="8" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="I224" s="5" t="s">
         <v>273</v>
@@ -12371,18 +12347,18 @@
         <v>0</v>
       </c>
       <c r="K224" s="5" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="225">
       <c r="A225" s="5" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="B225" s="6" t="n">
         <v>201</v>
       </c>
       <c r="C225" s="22" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="D225" s="5" t="s">
         <v>14</v>
@@ -12394,10 +12370,10 @@
         <v>114</v>
       </c>
       <c r="G225" s="5" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="H225" s="8" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="I225" s="5" t="s">
         <v>273</v>
@@ -12406,18 +12382,18 @@
         <v>0</v>
       </c>
       <c r="K225" s="5" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="226">
       <c r="A226" s="5" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="B226" s="8" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="C226" s="11" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="D226" s="5" t="s">
         <v>90</v>
@@ -12429,24 +12405,24 @@
         <v>125</v>
       </c>
       <c r="G226" s="5" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="H226" s="8" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="I226" s="5" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="J226" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K226" s="5" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="227">
       <c r="A227" s="8" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="B227" s="11"/>
       <c r="C227" s="11"/>
@@ -12458,12 +12434,12 @@
       <c r="I227" s="11"/>
       <c r="J227" s="11"/>
       <c r="K227" s="8" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="228">
       <c r="A228" s="33" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="B228" s="33"/>
       <c r="C228" s="33"/>
@@ -12478,13 +12454,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32.1" outlineLevel="0" r="229">
       <c r="A229" s="5" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="B229" s="6" t="n">
         <v>14</v>
       </c>
       <c r="C229" s="5" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="D229" s="5" t="s">
         <v>14</v>
@@ -12493,7 +12469,7 @@
         <v>0</v>
       </c>
       <c r="F229" s="5" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="G229" s="5" t="s">
         <v>273</v>
@@ -12502,27 +12478,27 @@
         <v>273</v>
       </c>
       <c r="I229" s="8" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="J229" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K229" s="5" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="230">
       <c r="A230" s="8" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="B230" s="8" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="C230" s="8" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="D230" s="8" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="E230" s="12" t="n">
         <v>0</v>
@@ -12534,7 +12510,7 @@
         <v>273</v>
       </c>
       <c r="H230" s="8" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="I230" s="8" t="s">
         <v>273</v>
@@ -12543,21 +12519,21 @@
         <v>0</v>
       </c>
       <c r="K230" s="8" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="231">
       <c r="A231" s="8" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="B231" s="8" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="C231" s="8" t="s">
         <v>270</v>
       </c>
       <c r="D231" s="8" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="E231" s="12" t="n">
         <v>0</v>
@@ -12572,24 +12548,24 @@
         <v>273</v>
       </c>
       <c r="I231" s="8" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="J231" s="14" t="n">
         <v>0</v>
       </c>
       <c r="K231" s="8" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32.1" outlineLevel="0" r="232">
       <c r="A232" s="5" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="B232" s="6" t="n">
         <v>14</v>
       </c>
       <c r="C232" s="5" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="D232" s="5" t="s">
         <v>30</v>
@@ -12604,21 +12580,21 @@
         <v>273</v>
       </c>
       <c r="H232" s="5" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="I232" s="8" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="J232" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K232" s="5" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="233">
       <c r="A233" s="5" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="B233" s="5" t="s">
         <v>21</v>
@@ -12627,13 +12603,13 @@
         <v>270</v>
       </c>
       <c r="D233" s="5" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="E233" s="7" t="n">
         <v>0</v>
       </c>
       <c r="F233" s="5" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="G233" s="5" t="s">
         <v>273</v>
@@ -12642,18 +12618,18 @@
         <v>273</v>
       </c>
       <c r="I233" s="5" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="J233" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K233" s="5" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="234">
       <c r="A234" s="33" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="B234" s="33"/>
       <c r="C234" s="33"/>
@@ -12668,13 +12644,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="235">
       <c r="A235" s="5" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="B235" s="5" t="s">
+        <v>949</v>
+      </c>
+      <c r="C235" s="5" t="s">
         <v>948</v>
-      </c>
-      <c r="C235" s="5" t="s">
-        <v>947</v>
       </c>
       <c r="D235" s="5" t="s">
         <v>97</v>
@@ -12683,7 +12659,7 @@
         <v>0</v>
       </c>
       <c r="F235" s="5" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="G235" s="5" t="s">
         <v>273</v>
@@ -12692,24 +12668,24 @@
         <v>273</v>
       </c>
       <c r="I235" s="5" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="J235" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K235" s="5" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="236">
       <c r="A236" s="5" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="B236" s="5" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="C236" s="19" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="D236" s="5" t="s">
         <v>90</v>
@@ -12724,27 +12700,27 @@
         <v>273</v>
       </c>
       <c r="H236" s="5" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="I236" s="8" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="J236" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K236" s="5" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="237">
       <c r="A237" s="11" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="B237" s="8" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="C237" s="11" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="D237" s="8" t="s">
         <v>14</v>
@@ -12753,7 +12729,7 @@
         <v>1</v>
       </c>
       <c r="F237" s="8" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="G237" s="8" t="s">
         <v>273</v>
@@ -12762,33 +12738,33 @@
         <v>273</v>
       </c>
       <c r="I237" s="8" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="J237" s="14" t="n">
         <v>0</v>
       </c>
       <c r="K237" s="8" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="238">
       <c r="A238" s="5" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="B238" s="5" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="C238" s="13" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="D238" s="5" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="E238" s="6" t="n">
         <v>1</v>
       </c>
       <c r="F238" s="8" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="G238" s="5" t="s">
         <v>273</v>
@@ -12797,33 +12773,33 @@
         <v>273</v>
       </c>
       <c r="I238" s="5" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="J238" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K238" s="5" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="239">
       <c r="A239" s="8" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B239" s="8" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C239" s="8" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="D239" s="8" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="E239" s="12" t="n">
         <v>0</v>
       </c>
       <c r="F239" s="8" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="G239" s="8" t="s">
         <v>273</v>
@@ -12832,33 +12808,33 @@
         <v>273</v>
       </c>
       <c r="I239" s="8" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="J239" s="14" t="n">
         <v>0</v>
       </c>
       <c r="K239" s="8" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="240">
       <c r="A240" s="8" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="B240" s="8" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C240" s="8" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="D240" s="8" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="E240" s="12" t="n">
         <v>0</v>
       </c>
       <c r="F240" s="8" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="G240" s="8" t="s">
         <v>273</v>
@@ -12867,33 +12843,33 @@
         <v>273</v>
       </c>
       <c r="I240" s="8" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="J240" s="14" t="n">
         <v>0</v>
       </c>
       <c r="K240" s="8" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="241">
       <c r="A241" s="5" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="B241" s="5" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C241" s="5" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="D241" s="5" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="E241" s="7" t="n">
         <v>0</v>
       </c>
       <c r="F241" s="5" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="G241" s="5" t="s">
         <v>273</v>
@@ -12902,33 +12878,33 @@
         <v>273</v>
       </c>
       <c r="I241" s="5" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="J241" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K241" s="5" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="242">
       <c r="A242" s="8" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B242" s="8" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C242" s="8" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="D242" s="8" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="E242" s="12" t="n">
         <v>0</v>
       </c>
       <c r="F242" s="8" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="G242" s="8" t="s">
         <v>273</v>
@@ -12937,33 +12913,33 @@
         <v>273</v>
       </c>
       <c r="I242" s="8" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="J242" s="14" t="n">
         <v>0</v>
       </c>
       <c r="K242" s="8" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="243">
       <c r="A243" s="8" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="B243" s="8" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C243" s="8" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="D243" s="8" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="E243" s="12" t="n">
         <v>0</v>
       </c>
       <c r="F243" s="8" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="G243" s="8" t="s">
         <v>273</v>
@@ -12972,33 +12948,33 @@
         <v>273</v>
       </c>
       <c r="I243" s="8" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="J243" s="14" t="n">
         <v>0</v>
       </c>
       <c r="K243" s="8" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="244">
       <c r="A244" s="8" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="B244" s="8" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C244" s="8" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="D244" s="8" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="E244" s="12" t="n">
         <v>0</v>
       </c>
       <c r="F244" s="8" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="G244" s="8" t="s">
         <v>273</v>
@@ -13007,33 +12983,33 @@
         <v>273</v>
       </c>
       <c r="I244" s="8" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="J244" s="14" t="n">
         <v>0</v>
       </c>
       <c r="K244" s="8" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="245">
       <c r="A245" s="8" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="B245" s="8" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C245" s="8" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="D245" s="8" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="E245" s="12" t="n">
         <v>0</v>
       </c>
       <c r="F245" s="8" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="G245" s="8" t="s">
         <v>273</v>
@@ -13042,29 +13018,29 @@
         <v>273</v>
       </c>
       <c r="I245" s="8" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="J245" s="14" t="n">
         <v>0</v>
       </c>
       <c r="K245" s="8" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="246">
-      <c r="A246" s="39" t="s">
-        <v>977</v>
-      </c>
-      <c r="B246" s="39"/>
-      <c r="C246" s="39"/>
-      <c r="D246" s="39"/>
-      <c r="E246" s="39"/>
-      <c r="F246" s="39"/>
-      <c r="G246" s="39"/>
-      <c r="H246" s="39"/>
-      <c r="I246" s="39"/>
-      <c r="J246" s="39"/>
-      <c r="K246" s="39"/>
+      <c r="A246" s="34" t="s">
+        <v>978</v>
+      </c>
+      <c r="B246" s="34"/>
+      <c r="C246" s="34"/>
+      <c r="D246" s="34"/>
+      <c r="E246" s="34"/>
+      <c r="F246" s="34"/>
+      <c r="G246" s="34"/>
+      <c r="H246" s="34"/>
+      <c r="I246" s="34"/>
+      <c r="J246" s="34"/>
+      <c r="K246" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="35">

</xml_diff>

<commit_message>
Update SBs in source SITs.
</commit_message>
<xml_diff>
--- a/sits/msit_feds.xlsx
+++ b/sits/msit_feds.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Table 1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Table 1'!$A$1:$K$246</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Table 1'!$A$1:$K$247</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1815" uniqueCount="979">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1824" uniqueCount="982">
   <si>
     <t>Designation</t>
   </si>
@@ -4239,6 +4239,48 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">36(24)</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="MS Gothic"/>
+        <charset val="1"/>
+        <family val="3"/>
+        <sz val="9"/>
+      </rPr>
+      <t xml:space="preserve">◆</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <sz val="9"/>
+      </rPr>
+      <t xml:space="preserve">/18(12)</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="MS Gothic"/>
+        <charset val="1"/>
+        <family val="3"/>
+        <sz val="9"/>
+      </rPr>
+      <t xml:space="preserve">◆</t>
+    </r>
+  </si>
+  <si>
+    <t>SB(1)</t>
+  </si>
+  <si>
+    <t>From BATS: 30+12</t>
+  </si>
+  <si>
+    <t>Starbase. See (433.41), (441.0), and
+(510.3)</t>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">36(18H12)</t>
     </r>
     <r>
@@ -4271,14 +4313,10 @@
     </r>
   </si>
   <si>
-    <t>SB(1)</t>
-  </si>
-  <si>
     <t>From BATS: 30+6</t>
   </si>
   <si>
-    <t>Starbase. See (433.41), (441.0), and
-(510.3)</t>
+    <t>Fed Starbase after Y181. See (433.41), (502.9).</t>
   </si>
   <si>
     <t>Ftr-Module</t>
@@ -5150,10 +5188,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K246"/>
+  <dimension ref="A1:K247"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A97" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="L110" activeCellId="0" pane="topLeft" sqref="L110"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A212" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="H214" activeCellId="0" pane="topLeft" sqref="H214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -12080,14 +12118,14 @@
       <c r="C217" s="22" t="s">
         <v>886</v>
       </c>
-      <c r="D217" s="5" t="s">
-        <v>14</v>
+      <c r="D217" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="E217" s="7" t="n">
         <v>10</v>
       </c>
       <c r="F217" s="5" t="s">
-        <v>137</v>
+        <v>308</v>
       </c>
       <c r="G217" s="5" t="s">
         <v>887</v>
@@ -12105,59 +12143,59 @@
         <v>889</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="218">
-      <c r="A218" s="8" t="s">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="218">
+      <c r="A218" s="5" t="s">
+        <v>884</v>
+      </c>
+      <c r="B218" s="5" t="s">
+        <v>885</v>
+      </c>
+      <c r="C218" s="22" t="s">
         <v>890</v>
       </c>
-      <c r="B218" s="12" t="n">
-        <v>4</v>
-      </c>
-      <c r="C218" s="11" t="s">
+      <c r="D218" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E218" s="7" t="n">
+        <v>10</v>
+      </c>
+      <c r="F218" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="G218" s="5" t="s">
+        <v>887</v>
+      </c>
+      <c r="H218" s="5" t="s">
         <v>891</v>
       </c>
-      <c r="D218" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E218" s="12" t="n">
+      <c r="I218" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="J218" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="F218" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="G218" s="8" t="s">
-        <v>273</v>
-      </c>
-      <c r="H218" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I218" s="8" t="s">
+      <c r="K218" s="8" t="s">
         <v>892</v>
-      </c>
-      <c r="J218" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="K218" s="8" t="s">
-        <v>893</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="219">
       <c r="A219" s="8" t="s">
+        <v>893</v>
+      </c>
+      <c r="B219" s="12" t="n">
+        <v>4</v>
+      </c>
+      <c r="C219" s="11" t="s">
         <v>894</v>
       </c>
-      <c r="B219" s="8" t="s">
-        <v>801</v>
-      </c>
-      <c r="C219" s="13" t="s">
-        <v>895</v>
-      </c>
       <c r="D219" s="8" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="E219" s="12" t="n">
         <v>0</v>
       </c>
       <c r="F219" s="8" t="s">
-        <v>57</v>
+        <v>149</v>
       </c>
       <c r="G219" s="8" t="s">
         <v>273</v>
@@ -12166,211 +12204,211 @@
         <v>17</v>
       </c>
       <c r="I219" s="8" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="J219" s="14" t="n">
         <v>0</v>
       </c>
       <c r="K219" s="8" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="220">
+      <c r="A220" s="8" t="s">
+        <v>897</v>
+      </c>
+      <c r="B220" s="8" t="s">
+        <v>801</v>
+      </c>
+      <c r="C220" s="13" t="s">
+        <v>898</v>
+      </c>
+      <c r="D220" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E220" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F220" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G220" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="H220" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I220" s="8" t="s">
+        <v>899</v>
+      </c>
+      <c r="J220" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K220" s="8" t="s">
         <v>804</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="220">
-      <c r="A220" s="5" t="s">
-        <v>897</v>
-      </c>
-      <c r="B220" s="6" t="n">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="221">
+      <c r="A221" s="5" t="s">
+        <v>900</v>
+      </c>
+      <c r="B221" s="6" t="n">
         <v>47</v>
       </c>
-      <c r="C220" s="11" t="s">
-        <v>898</v>
-      </c>
-      <c r="D220" s="5" t="s">
+      <c r="C221" s="11" t="s">
+        <v>901</v>
+      </c>
+      <c r="D221" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="E220" s="7" t="n">
+      <c r="E221" s="7" t="n">
         <v>9</v>
       </c>
-      <c r="F220" s="5" t="s">
+      <c r="F221" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="G220" s="5" t="s">
-        <v>899</v>
-      </c>
-      <c r="H220" s="8" t="s">
-        <v>900</v>
-      </c>
-      <c r="I220" s="5" t="s">
-        <v>901</v>
-      </c>
-      <c r="J220" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="K220" s="5" t="s">
+      <c r="G221" s="5" t="s">
         <v>902</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="221">
-      <c r="A221" s="8" t="s">
+      <c r="H221" s="8" t="s">
         <v>903</v>
       </c>
-      <c r="B221" s="6" t="n">
-        <v>17</v>
-      </c>
-      <c r="C221" s="19" t="s">
+      <c r="I221" s="5" t="s">
         <v>904</v>
-      </c>
-      <c r="D221" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E221" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F221" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="G221" s="5" t="s">
-        <v>273</v>
-      </c>
-      <c r="H221" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I221" s="5" t="s">
-        <v>905</v>
       </c>
       <c r="J221" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K221" s="5" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="222">
+      <c r="A222" s="8" t="s">
         <v>906</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32.1" outlineLevel="0" r="222">
-      <c r="A222" s="5" t="s">
+      <c r="B222" s="6" t="n">
+        <v>17</v>
+      </c>
+      <c r="C222" s="19" t="s">
         <v>907</v>
-      </c>
-      <c r="B222" s="6" t="n">
-        <v>202</v>
-      </c>
-      <c r="C222" s="11" t="s">
-        <v>908</v>
       </c>
       <c r="D222" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E222" s="7" t="n">
-        <v>10</v>
+      <c r="E222" s="6" t="n">
+        <v>0</v>
       </c>
       <c r="F222" s="5" t="s">
-        <v>114</v>
+        <v>78</v>
       </c>
       <c r="G222" s="5" t="s">
-        <v>909</v>
-      </c>
-      <c r="H222" s="8" t="s">
-        <v>910</v>
+        <v>273</v>
+      </c>
+      <c r="H222" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="I222" s="5" t="s">
-        <v>273</v>
+        <v>908</v>
       </c>
       <c r="J222" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K222" s="5" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32.1" outlineLevel="0" r="223">
+      <c r="A223" s="5" t="s">
+        <v>910</v>
+      </c>
+      <c r="B223" s="6" t="n">
+        <v>202</v>
+      </c>
+      <c r="C223" s="11" t="s">
         <v>911</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32.1" outlineLevel="0" r="223">
-      <c r="A223" s="1" t="s">
+      <c r="D223" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E223" s="7" t="n">
+        <v>10</v>
+      </c>
+      <c r="F223" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="G223" s="5" t="s">
+        <v>912</v>
+      </c>
+      <c r="H223" s="8" t="s">
+        <v>913</v>
+      </c>
+      <c r="I223" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="J223" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="B223" s="2" t="s">
+      <c r="K223" s="5" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32.1" outlineLevel="0" r="224">
+      <c r="A224" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B224" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C223" s="1" t="s">
+      <c r="C224" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D223" s="1" t="s">
+      <c r="D224" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E223" s="1" t="s">
+      <c r="E224" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F223" s="1" t="s">
+      <c r="F224" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G223" s="1" t="s">
+      <c r="G224" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H223" s="1" t="s">
+      <c r="H224" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I223" s="1" t="s">
+      <c r="I224" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J223" s="1" t="s">
+      <c r="J224" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K223" s="1" t="s">
+      <c r="K224" s="1" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="224">
-      <c r="A224" s="5" t="s">
-        <v>912</v>
-      </c>
-      <c r="B224" s="5" t="s">
-        <v>913</v>
-      </c>
-      <c r="C224" s="11" t="s">
-        <v>914</v>
-      </c>
-      <c r="D224" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E224" s="7" t="n">
-        <v>9</v>
-      </c>
-      <c r="F224" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G224" s="5" t="s">
-        <v>869</v>
-      </c>
-      <c r="H224" s="8" t="s">
-        <v>915</v>
-      </c>
-      <c r="I224" s="5" t="s">
-        <v>273</v>
-      </c>
-      <c r="J224" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="K224" s="5" t="s">
-        <v>871</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="225">
       <c r="A225" s="5" t="s">
+        <v>915</v>
+      </c>
+      <c r="B225" s="5" t="s">
         <v>916</v>
       </c>
-      <c r="B225" s="6" t="n">
-        <v>201</v>
-      </c>
-      <c r="C225" s="22" t="s">
+      <c r="C225" s="11" t="s">
         <v>917</v>
       </c>
       <c r="D225" s="5" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E225" s="7" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F225" s="5" t="s">
         <v>114</v>
       </c>
       <c r="G225" s="5" t="s">
-        <v>887</v>
+        <v>869</v>
       </c>
       <c r="H225" s="8" t="s">
         <v>918</v>
@@ -12382,155 +12420,155 @@
         <v>0</v>
       </c>
       <c r="K225" s="5" t="s">
-        <v>919</v>
+        <v>871</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="226">
       <c r="A226" s="5" t="s">
+        <v>919</v>
+      </c>
+      <c r="B226" s="6" t="n">
+        <v>201</v>
+      </c>
+      <c r="C226" s="22" t="s">
         <v>920</v>
       </c>
-      <c r="B226" s="8" t="s">
+      <c r="D226" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E226" s="7" t="n">
+        <v>11</v>
+      </c>
+      <c r="F226" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="G226" s="5" t="s">
+        <v>887</v>
+      </c>
+      <c r="H226" s="8" t="s">
         <v>921</v>
       </c>
-      <c r="C226" s="11" t="s">
-        <v>922</v>
-      </c>
-      <c r="D226" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E226" s="7" t="n">
-        <v>10</v>
-      </c>
-      <c r="F226" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="G226" s="5" t="s">
-        <v>899</v>
-      </c>
-      <c r="H226" s="8" t="s">
-        <v>923</v>
-      </c>
       <c r="I226" s="5" t="s">
-        <v>901</v>
+        <v>273</v>
       </c>
       <c r="J226" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K226" s="5" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="227">
+      <c r="A227" s="5" t="s">
+        <v>923</v>
+      </c>
+      <c r="B227" s="8" t="s">
         <v>924</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="227">
-      <c r="A227" s="8" t="s">
+      <c r="C227" s="11" t="s">
         <v>925</v>
       </c>
-      <c r="B227" s="11"/>
-      <c r="C227" s="11"/>
-      <c r="D227" s="11"/>
-      <c r="E227" s="11"/>
-      <c r="F227" s="11"/>
-      <c r="G227" s="11"/>
-      <c r="H227" s="11"/>
-      <c r="I227" s="11"/>
-      <c r="J227" s="11"/>
-      <c r="K227" s="8" t="s">
+      <c r="D227" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E227" s="7" t="n">
+        <v>10</v>
+      </c>
+      <c r="F227" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="G227" s="5" t="s">
+        <v>902</v>
+      </c>
+      <c r="H227" s="8" t="s">
         <v>926</v>
       </c>
+      <c r="I227" s="5" t="s">
+        <v>904</v>
+      </c>
+      <c r="J227" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K227" s="5" t="s">
+        <v>927</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="228">
-      <c r="A228" s="33" t="s">
-        <v>927</v>
-      </c>
-      <c r="B228" s="33"/>
-      <c r="C228" s="33"/>
-      <c r="D228" s="33"/>
-      <c r="E228" s="33"/>
-      <c r="F228" s="33"/>
-      <c r="G228" s="33"/>
-      <c r="H228" s="33"/>
-      <c r="I228" s="33"/>
-      <c r="J228" s="33"/>
-      <c r="K228" s="33"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32.1" outlineLevel="0" r="229">
-      <c r="A229" s="5" t="s">
+      <c r="A228" s="8" t="s">
         <v>928</v>
       </c>
-      <c r="B229" s="6" t="n">
+      <c r="B228" s="11"/>
+      <c r="C228" s="11"/>
+      <c r="D228" s="11"/>
+      <c r="E228" s="11"/>
+      <c r="F228" s="11"/>
+      <c r="G228" s="11"/>
+      <c r="H228" s="11"/>
+      <c r="I228" s="11"/>
+      <c r="J228" s="11"/>
+      <c r="K228" s="8" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="229">
+      <c r="A229" s="33" t="s">
+        <v>930</v>
+      </c>
+      <c r="B229" s="33"/>
+      <c r="C229" s="33"/>
+      <c r="D229" s="33"/>
+      <c r="E229" s="33"/>
+      <c r="F229" s="33"/>
+      <c r="G229" s="33"/>
+      <c r="H229" s="33"/>
+      <c r="I229" s="33"/>
+      <c r="J229" s="33"/>
+      <c r="K229" s="33"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32.1" outlineLevel="0" r="230">
+      <c r="A230" s="5" t="s">
+        <v>931</v>
+      </c>
+      <c r="B230" s="6" t="n">
         <v>14</v>
       </c>
-      <c r="C229" s="5" t="s">
-        <v>929</v>
-      </c>
-      <c r="D229" s="5" t="s">
+      <c r="C230" s="5" t="s">
+        <v>932</v>
+      </c>
+      <c r="D230" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E229" s="7" t="n">
+      <c r="E230" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="F229" s="5" t="s">
+      <c r="F230" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="G229" s="5" t="s">
+      <c r="G230" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="H229" s="5" t="s">
+      <c r="H230" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="I229" s="8" t="s">
-        <v>930</v>
-      </c>
-      <c r="J229" s="9" t="n">
+      <c r="I230" s="8" t="s">
+        <v>933</v>
+      </c>
+      <c r="J230" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="K229" s="5" t="s">
-        <v>931</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="230">
-      <c r="A230" s="8" t="s">
-        <v>932</v>
-      </c>
-      <c r="B230" s="8" t="s">
-        <v>801</v>
-      </c>
-      <c r="C230" s="8" t="s">
-        <v>933</v>
-      </c>
-      <c r="D230" s="8" t="s">
-        <v>642</v>
-      </c>
-      <c r="E230" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F230" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="G230" s="8" t="s">
-        <v>273</v>
-      </c>
-      <c r="H230" s="8" t="s">
+      <c r="K230" s="5" t="s">
         <v>934</v>
-      </c>
-      <c r="I230" s="8" t="s">
-        <v>273</v>
-      </c>
-      <c r="J230" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="K230" s="8" t="s">
-        <v>935</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="231">
       <c r="A231" s="8" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="B231" s="8" t="s">
         <v>801</v>
       </c>
       <c r="C231" s="8" t="s">
-        <v>270</v>
+        <v>936</v>
       </c>
       <c r="D231" s="8" t="s">
         <v>642</v>
@@ -12545,10 +12583,10 @@
         <v>273</v>
       </c>
       <c r="H231" s="8" t="s">
+        <v>937</v>
+      </c>
+      <c r="I231" s="8" t="s">
         <v>273</v>
-      </c>
-      <c r="I231" s="8" t="s">
-        <v>937</v>
       </c>
       <c r="J231" s="14" t="n">
         <v>0</v>
@@ -12557,67 +12595,67 @@
         <v>938</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32.1" outlineLevel="0" r="232">
-      <c r="A232" s="5" t="s">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="232">
+      <c r="A232" s="8" t="s">
         <v>939</v>
       </c>
-      <c r="B232" s="6" t="n">
+      <c r="B232" s="8" t="s">
+        <v>801</v>
+      </c>
+      <c r="C232" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="D232" s="8" t="s">
+        <v>642</v>
+      </c>
+      <c r="E232" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F232" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="G232" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="H232" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="I232" s="8" t="s">
+        <v>940</v>
+      </c>
+      <c r="J232" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K232" s="8" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32.1" outlineLevel="0" r="233">
+      <c r="A233" s="5" t="s">
+        <v>942</v>
+      </c>
+      <c r="B233" s="6" t="n">
         <v>14</v>
       </c>
-      <c r="C232" s="5" t="s">
-        <v>940</v>
-      </c>
-      <c r="D232" s="5" t="s">
+      <c r="C233" s="5" t="s">
+        <v>943</v>
+      </c>
+      <c r="D233" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="E232" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F232" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="G232" s="5" t="s">
-        <v>273</v>
-      </c>
-      <c r="H232" s="5" t="s">
-        <v>941</v>
-      </c>
-      <c r="I232" s="8" t="s">
-        <v>942</v>
-      </c>
-      <c r="J232" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="K232" s="5" t="s">
-        <v>943</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="233">
-      <c r="A233" s="5" t="s">
-        <v>944</v>
-      </c>
-      <c r="B233" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C233" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="D233" s="5" t="s">
-        <v>642</v>
       </c>
       <c r="E233" s="7" t="n">
         <v>0</v>
       </c>
       <c r="F233" s="5" t="s">
-        <v>687</v>
+        <v>38</v>
       </c>
       <c r="G233" s="5" t="s">
         <v>273</v>
       </c>
       <c r="H233" s="5" t="s">
-        <v>273</v>
-      </c>
-      <c r="I233" s="5" t="s">
+        <v>944</v>
+      </c>
+      <c r="I233" s="8" t="s">
         <v>945</v>
       </c>
       <c r="J233" s="9" t="n">
@@ -12627,205 +12665,205 @@
         <v>946</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="234">
-      <c r="A234" s="33" t="s">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="234">
+      <c r="A234" s="5" t="s">
         <v>947</v>
       </c>
-      <c r="B234" s="33"/>
-      <c r="C234" s="33"/>
-      <c r="D234" s="33"/>
-      <c r="E234" s="33"/>
-      <c r="F234" s="33"/>
-      <c r="G234" s="33"/>
-      <c r="H234" s="33"/>
-      <c r="I234" s="33"/>
-      <c r="J234" s="33"/>
-      <c r="K234" s="33"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="235">
-      <c r="A235" s="5" t="s">
+      <c r="B234" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C234" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="D234" s="5" t="s">
+        <v>642</v>
+      </c>
+      <c r="E234" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F234" s="5" t="s">
+        <v>687</v>
+      </c>
+      <c r="G234" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="H234" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="I234" s="5" t="s">
         <v>948</v>
       </c>
-      <c r="B235" s="5" t="s">
+      <c r="J234" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K234" s="5" t="s">
         <v>949</v>
       </c>
-      <c r="C235" s="5" t="s">
-        <v>948</v>
-      </c>
-      <c r="D235" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="E235" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F235" s="5" t="s">
-        <v>732</v>
-      </c>
-      <c r="G235" s="5" t="s">
-        <v>273</v>
-      </c>
-      <c r="H235" s="5" t="s">
-        <v>273</v>
-      </c>
-      <c r="I235" s="5" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="235">
+      <c r="A235" s="33" t="s">
         <v>950</v>
       </c>
-      <c r="J235" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="K235" s="5" t="s">
-        <v>948</v>
-      </c>
+      <c r="B235" s="33"/>
+      <c r="C235" s="33"/>
+      <c r="D235" s="33"/>
+      <c r="E235" s="33"/>
+      <c r="F235" s="33"/>
+      <c r="G235" s="33"/>
+      <c r="H235" s="33"/>
+      <c r="I235" s="33"/>
+      <c r="J235" s="33"/>
+      <c r="K235" s="33"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="236">
       <c r="A236" s="5" t="s">
         <v>951</v>
       </c>
       <c r="B236" s="5" t="s">
-        <v>801</v>
-      </c>
-      <c r="C236" s="19" t="s">
+        <v>952</v>
+      </c>
+      <c r="C236" s="5" t="s">
         <v>951</v>
       </c>
       <c r="D236" s="5" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="E236" s="7" t="n">
         <v>0</v>
       </c>
       <c r="F236" s="5" t="s">
-        <v>278</v>
+        <v>732</v>
       </c>
       <c r="G236" s="5" t="s">
         <v>273</v>
       </c>
       <c r="H236" s="5" t="s">
-        <v>801</v>
-      </c>
-      <c r="I236" s="8" t="s">
-        <v>952</v>
+        <v>273</v>
+      </c>
+      <c r="I236" s="5" t="s">
+        <v>953</v>
       </c>
       <c r="J236" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K236" s="5" t="s">
-        <v>953</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="237">
-      <c r="A237" s="11" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="237">
+      <c r="A237" s="5" t="s">
         <v>954</v>
       </c>
-      <c r="B237" s="8" t="s">
+      <c r="B237" s="5" t="s">
         <v>801</v>
       </c>
-      <c r="C237" s="11" t="s">
+      <c r="C237" s="19" t="s">
         <v>954</v>
       </c>
-      <c r="D237" s="8" t="s">
+      <c r="D237" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E237" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F237" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="G237" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="H237" s="5" t="s">
+        <v>801</v>
+      </c>
+      <c r="I237" s="8" t="s">
+        <v>955</v>
+      </c>
+      <c r="J237" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K237" s="5" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="238">
+      <c r="A238" s="11" t="s">
+        <v>957</v>
+      </c>
+      <c r="B238" s="8" t="s">
+        <v>801</v>
+      </c>
+      <c r="C238" s="11" t="s">
+        <v>957</v>
+      </c>
+      <c r="D238" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E237" s="12" t="n">
+      <c r="E238" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="F237" s="8" t="s">
-        <v>955</v>
-      </c>
-      <c r="G237" s="8" t="s">
+      <c r="F238" s="8" t="s">
+        <v>958</v>
+      </c>
+      <c r="G238" s="8" t="s">
         <v>273</v>
       </c>
-      <c r="H237" s="8" t="s">
+      <c r="H238" s="8" t="s">
         <v>273</v>
       </c>
-      <c r="I237" s="8" t="s">
-        <v>956</v>
-      </c>
-      <c r="J237" s="14" t="n">
+      <c r="I238" s="8" t="s">
+        <v>959</v>
+      </c>
+      <c r="J238" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="K237" s="8" t="s">
-        <v>957</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="238">
-      <c r="A238" s="5" t="s">
-        <v>958</v>
-      </c>
-      <c r="B238" s="5" t="s">
+      <c r="K238" s="8" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="239">
+      <c r="A239" s="5" t="s">
+        <v>961</v>
+      </c>
+      <c r="B239" s="5" t="s">
         <v>801</v>
       </c>
-      <c r="C238" s="13" t="s">
-        <v>959</v>
-      </c>
-      <c r="D238" s="5" t="s">
+      <c r="C239" s="13" t="s">
+        <v>962</v>
+      </c>
+      <c r="D239" s="5" t="s">
         <v>642</v>
       </c>
-      <c r="E238" s="6" t="n">
+      <c r="E239" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="F238" s="8" t="s">
-        <v>960</v>
-      </c>
-      <c r="G238" s="5" t="s">
+      <c r="F239" s="8" t="s">
+        <v>963</v>
+      </c>
+      <c r="G239" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="H238" s="5" t="s">
+      <c r="H239" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="I238" s="5" t="s">
-        <v>961</v>
-      </c>
-      <c r="J238" s="9" t="n">
+      <c r="I239" s="5" t="s">
+        <v>964</v>
+      </c>
+      <c r="J239" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="K238" s="5" t="s">
-        <v>962</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="239">
-      <c r="A239" s="8" t="s">
-        <v>963</v>
-      </c>
-      <c r="B239" s="8" t="s">
-        <v>964</v>
-      </c>
-      <c r="C239" s="8" t="s">
+      <c r="K239" s="5" t="s">
         <v>965</v>
-      </c>
-      <c r="D239" s="8" t="s">
-        <v>642</v>
-      </c>
-      <c r="E239" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F239" s="8" t="s">
-        <v>966</v>
-      </c>
-      <c r="G239" s="8" t="s">
-        <v>273</v>
-      </c>
-      <c r="H239" s="8" t="s">
-        <v>273</v>
-      </c>
-      <c r="I239" s="8" t="s">
-        <v>967</v>
-      </c>
-      <c r="J239" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="K239" s="8" t="s">
-        <v>968</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="240">
       <c r="A240" s="8" t="s">
-        <v>969</v>
+        <v>966</v>
       </c>
       <c r="B240" s="8" t="s">
-        <v>964</v>
+        <v>967</v>
       </c>
       <c r="C240" s="8" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="D240" s="8" t="s">
         <v>642</v>
@@ -12834,7 +12872,7 @@
         <v>0</v>
       </c>
       <c r="F240" s="8" t="s">
-        <v>966</v>
+        <v>969</v>
       </c>
       <c r="G240" s="8" t="s">
         <v>273</v>
@@ -12843,94 +12881,94 @@
         <v>273</v>
       </c>
       <c r="I240" s="8" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="J240" s="14" t="n">
         <v>0</v>
       </c>
       <c r="K240" s="8" t="s">
-        <v>968</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="241">
-      <c r="A241" s="5" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="241">
+      <c r="A241" s="8" t="s">
         <v>972</v>
       </c>
-      <c r="B241" s="5" t="s">
-        <v>964</v>
-      </c>
-      <c r="C241" s="5" t="s">
+      <c r="B241" s="8" t="s">
+        <v>967</v>
+      </c>
+      <c r="C241" s="8" t="s">
         <v>973</v>
       </c>
-      <c r="D241" s="5" t="s">
+      <c r="D241" s="8" t="s">
         <v>642</v>
       </c>
-      <c r="E241" s="7" t="n">
+      <c r="E241" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="F241" s="5" t="s">
-        <v>966</v>
-      </c>
-      <c r="G241" s="5" t="s">
+      <c r="F241" s="8" t="s">
+        <v>969</v>
+      </c>
+      <c r="G241" s="8" t="s">
         <v>273</v>
       </c>
-      <c r="H241" s="5" t="s">
+      <c r="H241" s="8" t="s">
         <v>273</v>
       </c>
-      <c r="I241" s="5" t="s">
+      <c r="I241" s="8" t="s">
+        <v>974</v>
+      </c>
+      <c r="J241" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K241" s="8" t="s">
         <v>971</v>
       </c>
-      <c r="J241" s="9" t="n">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="242">
+      <c r="A242" s="5" t="s">
+        <v>975</v>
+      </c>
+      <c r="B242" s="5" t="s">
+        <v>967</v>
+      </c>
+      <c r="C242" s="5" t="s">
+        <v>976</v>
+      </c>
+      <c r="D242" s="5" t="s">
+        <v>642</v>
+      </c>
+      <c r="E242" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="K241" s="5" t="s">
-        <v>968</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="242">
-      <c r="A242" s="8" t="s">
+      <c r="F242" s="5" t="s">
+        <v>969</v>
+      </c>
+      <c r="G242" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="H242" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="I242" s="5" t="s">
         <v>974</v>
       </c>
-      <c r="B242" s="8" t="s">
-        <v>964</v>
-      </c>
-      <c r="C242" s="8" t="s">
-        <v>965</v>
-      </c>
-      <c r="D242" s="8" t="s">
-        <v>642</v>
-      </c>
-      <c r="E242" s="12" t="n">
+      <c r="J242" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="F242" s="8" t="s">
-        <v>966</v>
-      </c>
-      <c r="G242" s="8" t="s">
-        <v>273</v>
-      </c>
-      <c r="H242" s="8" t="s">
-        <v>273</v>
-      </c>
-      <c r="I242" s="8" t="s">
-        <v>967</v>
-      </c>
-      <c r="J242" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="K242" s="8" t="s">
-        <v>968</v>
+      <c r="K242" s="5" t="s">
+        <v>971</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="243">
       <c r="A243" s="8" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="B243" s="8" t="s">
-        <v>964</v>
+        <v>967</v>
       </c>
       <c r="C243" s="8" t="s">
-        <v>965</v>
+        <v>968</v>
       </c>
       <c r="D243" s="8" t="s">
         <v>642</v>
@@ -12939,7 +12977,7 @@
         <v>0</v>
       </c>
       <c r="F243" s="8" t="s">
-        <v>966</v>
+        <v>969</v>
       </c>
       <c r="G243" s="8" t="s">
         <v>273</v>
@@ -12948,24 +12986,24 @@
         <v>273</v>
       </c>
       <c r="I243" s="8" t="s">
-        <v>967</v>
+        <v>970</v>
       </c>
       <c r="J243" s="14" t="n">
         <v>0</v>
       </c>
       <c r="K243" s="8" t="s">
-        <v>968</v>
+        <v>971</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="244">
       <c r="A244" s="8" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
       <c r="B244" s="8" t="s">
-        <v>964</v>
+        <v>967</v>
       </c>
       <c r="C244" s="8" t="s">
-        <v>965</v>
+        <v>968</v>
       </c>
       <c r="D244" s="8" t="s">
         <v>642</v>
@@ -12974,7 +13012,7 @@
         <v>0</v>
       </c>
       <c r="F244" s="8" t="s">
-        <v>966</v>
+        <v>969</v>
       </c>
       <c r="G244" s="8" t="s">
         <v>273</v>
@@ -12983,24 +13021,24 @@
         <v>273</v>
       </c>
       <c r="I244" s="8" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="J244" s="14" t="n">
         <v>0</v>
       </c>
       <c r="K244" s="8" t="s">
-        <v>968</v>
+        <v>971</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="245">
       <c r="A245" s="8" t="s">
-        <v>977</v>
+        <v>979</v>
       </c>
       <c r="B245" s="8" t="s">
-        <v>964</v>
+        <v>967</v>
       </c>
       <c r="C245" s="8" t="s">
-        <v>965</v>
+        <v>968</v>
       </c>
       <c r="D245" s="8" t="s">
         <v>642</v>
@@ -13009,7 +13047,7 @@
         <v>0</v>
       </c>
       <c r="F245" s="8" t="s">
-        <v>966</v>
+        <v>969</v>
       </c>
       <c r="G245" s="8" t="s">
         <v>273</v>
@@ -13018,29 +13056,64 @@
         <v>273</v>
       </c>
       <c r="I245" s="8" t="s">
-        <v>967</v>
+        <v>974</v>
       </c>
       <c r="J245" s="14" t="n">
         <v>0</v>
       </c>
       <c r="K245" s="8" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="246">
+      <c r="A246" s="8" t="s">
+        <v>980</v>
+      </c>
+      <c r="B246" s="8" t="s">
+        <v>967</v>
+      </c>
+      <c r="C246" s="8" t="s">
         <v>968</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="246">
-      <c r="A246" s="34" t="s">
-        <v>978</v>
-      </c>
-      <c r="B246" s="34"/>
-      <c r="C246" s="34"/>
-      <c r="D246" s="34"/>
-      <c r="E246" s="34"/>
-      <c r="F246" s="34"/>
-      <c r="G246" s="34"/>
-      <c r="H246" s="34"/>
-      <c r="I246" s="34"/>
-      <c r="J246" s="34"/>
-      <c r="K246" s="34"/>
+      <c r="D246" s="8" t="s">
+        <v>642</v>
+      </c>
+      <c r="E246" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F246" s="8" t="s">
+        <v>969</v>
+      </c>
+      <c r="G246" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="H246" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="I246" s="8" t="s">
+        <v>970</v>
+      </c>
+      <c r="J246" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K246" s="8" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="247">
+      <c r="A247" s="34" t="s">
+        <v>981</v>
+      </c>
+      <c r="B247" s="34"/>
+      <c r="C247" s="34"/>
+      <c r="D247" s="34"/>
+      <c r="E247" s="34"/>
+      <c r="F247" s="34"/>
+      <c r="G247" s="34"/>
+      <c r="H247" s="34"/>
+      <c r="I247" s="34"/>
+      <c r="J247" s="34"/>
+      <c r="K247" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="35">
@@ -13076,9 +13149,9 @@
     <mergeCell ref="A194:K194"/>
     <mergeCell ref="A206:K206"/>
     <mergeCell ref="A211:K211"/>
-    <mergeCell ref="A228:K228"/>
-    <mergeCell ref="A234:K234"/>
-    <mergeCell ref="A246:K246"/>
+    <mergeCell ref="A229:K229"/>
+    <mergeCell ref="A235:K235"/>
+    <mergeCell ref="A247:K247"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>